<commit_message>
design doc updated fully
</commit_message>
<xml_diff>
--- a/etc/term-2181-swen-261-11-d.xlsx
+++ b/etc/term-2181-swen-261-11-d.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="81">
   <si>
     <t>Instructions</t>
   </si>
@@ -251,6 +251,30 @@
   </si>
   <si>
     <t>Given a player wants to resign when they press the forfeit button then the game will end and the opponent will win.</t>
+  </si>
+  <si>
+    <t>ZM 10/26</t>
+  </si>
+  <si>
+    <t>NS  10/28</t>
+  </si>
+  <si>
+    <t>JK 10/29</t>
+  </si>
+  <si>
+    <t>SQ 10/31</t>
+  </si>
+  <si>
+    <t>SF 10/31</t>
+  </si>
+  <si>
+    <t>SQ 11/2</t>
+  </si>
+  <si>
+    <t>ZM 10/30</t>
+  </si>
+  <si>
+    <t>NS  11/17</t>
   </si>
 </sst>
 </file>
@@ -441,7 +465,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="48">
+  <dxfs count="38">
     <dxf>
       <fill>
         <patternFill>
@@ -453,6 +477,26 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -471,58 +515,42 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -575,16 +603,22 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -603,16 +637,42 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -631,86 +691,42 @@
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -779,20 +795,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1173,9 +1175,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V592"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="D42" sqref="D42"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1556,7 +1558,12 @@
       <c r="D19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="8"/>
+      <c r="E19" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="G19" s="8"/>
     </row>
     <row r="20" spans="1:22" ht="32" x14ac:dyDescent="0.2">
@@ -1567,7 +1574,12 @@
       <c r="D20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="8"/>
+      <c r="E20" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="G20" s="8"/>
     </row>
     <row r="21" spans="1:22" ht="32" x14ac:dyDescent="0.2">
@@ -1578,7 +1590,12 @@
       <c r="D21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="8"/>
+      <c r="E21" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="G21" s="8"/>
     </row>
     <row r="22" spans="1:22" ht="32" x14ac:dyDescent="0.2">
@@ -1589,7 +1606,12 @@
       <c r="D22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="8"/>
+      <c r="E22" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="G22" s="8"/>
     </row>
     <row r="23" spans="1:22" ht="32" x14ac:dyDescent="0.2">
@@ -1601,7 +1623,12 @@
       <c r="D23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="8"/>
+      <c r="E23" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="G23" s="8"/>
     </row>
     <row r="24" spans="1:22" ht="48" x14ac:dyDescent="0.2">
@@ -1615,8 +1642,12 @@
       <c r="D24" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="22"/>
+      <c r="E24" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>80</v>
+      </c>
       <c r="G24" s="25"/>
       <c r="H24" s="22"/>
       <c r="I24" s="26"/>
@@ -1645,7 +1676,12 @@
       <c r="D25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="8"/>
+      <c r="E25" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="22" t="s">
+        <v>80</v>
+      </c>
       <c r="G25" s="8"/>
     </row>
     <row r="26" spans="1:22" ht="80" x14ac:dyDescent="0.2">
@@ -1659,7 +1695,12 @@
       <c r="D26" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="8"/>
+      <c r="E26" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="22" t="s">
+        <v>80</v>
+      </c>
       <c r="G26" s="8"/>
     </row>
     <row r="27" spans="1:22" ht="48" x14ac:dyDescent="0.2">
@@ -1673,7 +1714,12 @@
       <c r="D27" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="8"/>
+      <c r="E27" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="22" t="s">
+        <v>80</v>
+      </c>
       <c r="G27" s="8"/>
     </row>
     <row r="28" spans="1:22" ht="64" x14ac:dyDescent="0.2">
@@ -1687,7 +1733,12 @@
       <c r="D28" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E28" s="8"/>
+      <c r="E28" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="G28" s="8"/>
     </row>
     <row r="29" spans="1:22" ht="32" x14ac:dyDescent="0.2">
@@ -1699,7 +1750,12 @@
       <c r="D29" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E29" s="8"/>
+      <c r="E29" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="G29" s="8"/>
     </row>
     <row r="30" spans="1:22" ht="96" x14ac:dyDescent="0.2">
@@ -1713,7 +1769,12 @@
       <c r="D30" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E30" s="8"/>
+      <c r="E30" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="G30" s="8"/>
     </row>
     <row r="31" spans="1:22" ht="32" x14ac:dyDescent="0.2">
@@ -1725,7 +1786,12 @@
       <c r="D31" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E31" s="8"/>
+      <c r="E31" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="G31" s="8"/>
     </row>
     <row r="32" spans="1:22" ht="64" x14ac:dyDescent="0.2">
@@ -1739,7 +1805,12 @@
       <c r="D32" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E32" s="8"/>
+      <c r="E32" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="G32" s="8"/>
     </row>
     <row r="33" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1751,7 +1822,12 @@
       <c r="D33" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E33" s="8"/>
+      <c r="E33" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="G33" s="8"/>
     </row>
     <row r="34" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1763,7 +1839,12 @@
       <c r="D34" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E34" s="8"/>
+      <c r="E34" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="G34" s="8"/>
     </row>
     <row r="35" spans="1:7" ht="80" x14ac:dyDescent="0.2">
@@ -1777,7 +1858,12 @@
       <c r="D35" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E35" s="8"/>
+      <c r="E35" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="G35" s="8"/>
     </row>
     <row r="36" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1789,7 +1875,12 @@
       <c r="D36" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E36" s="8"/>
+      <c r="E36" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>77</v>
+      </c>
       <c r="G36" s="8"/>
     </row>
     <row r="37" spans="1:7" ht="64" x14ac:dyDescent="0.2">
@@ -1803,7 +1894,12 @@
       <c r="D37" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E37" s="8"/>
+      <c r="E37" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="G37" s="8"/>
     </row>
     <row r="38" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1815,7 +1911,12 @@
       <c r="D38" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E38" s="8"/>
+      <c r="E38" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="G38" s="8"/>
     </row>
     <row r="39" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1827,7 +1928,12 @@
       <c r="D39" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E39" s="8"/>
+      <c r="E39" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="G39" s="8"/>
     </row>
     <row r="40" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1839,7 +1945,12 @@
       <c r="D40" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E40" s="8"/>
+      <c r="E40" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="G40" s="8"/>
     </row>
     <row r="41" spans="1:7" ht="32" x14ac:dyDescent="0.2">
@@ -1851,7 +1962,12 @@
       <c r="D41" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E41" s="8"/>
+      <c r="E41" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>78</v>
+      </c>
       <c r="G41" s="8"/>
     </row>
     <row r="42" spans="1:7" ht="48" x14ac:dyDescent="0.2">
@@ -1865,7 +1981,12 @@
       <c r="D42" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E42" s="8"/>
+      <c r="E42" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>76</v>
+      </c>
       <c r="G42" s="8"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -4619,24 +4740,24 @@
       <c r="G592" s="8"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:G592 E2:E592 C2:C592">
-    <cfRule type="cellIs" dxfId="15" priority="11" operator="equal">
+  <conditionalFormatting sqref="G2:G592 C2:C592 E2:E592">
+    <cfRule type="cellIs" dxfId="35" priority="11" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="12" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F592 H2:H592 D2:D592">
-    <cfRule type="expression" dxfId="13" priority="5" stopIfTrue="1">
+  <conditionalFormatting sqref="H2:H592 D2:D592 F2:F18 F24:F592">
+    <cfRule type="expression" dxfId="33" priority="5" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="6" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C592 E2:E592 G2:G592">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C592 G2:G592 E2:E592">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
didn't save the changes to acceptance test plan. Oops.
</commit_message>
<xml_diff>
--- a/etc/term-2181-swen-261-11-d.xlsx
+++ b/etc/term-2181-swen-261-11-d.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="102">
   <si>
     <t>Instructions</t>
   </si>
@@ -276,12 +276,658 @@
   <si>
     <t>NS  11/17</t>
   </si>
+  <si>
+    <t>King Crown</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I am playing a game </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I move a piece to hit the other side of the board </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I expect that piece to become a king.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I am playing a game </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I move a piece after I hit the other side of the board </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I expect that piece to stay a king.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I am playing a game </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> one of my pieces becomes a king </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I expect that piece to have a visible mark on it showing it is a king.</t>
+    </r>
+  </si>
+  <si>
+    <t>King Backwards</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I am playing a game </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> one of my pieces becomes a king </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I expect that piece to be able to move backwards.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">King Backwards Jump </t>
+  </si>
+  <si>
+    <t>Select AI Opponent</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that I am on the start a game screen </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I try to start a game </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I should be able to choose to play against the machine</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that I choose to play against the machine </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I start a game </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> my opponent should be an automated AI player</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> AI Detect Move</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that the opponent is an AI player </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> it is their turn </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> they should make valid moves in a reasonable time frame</t>
+    </r>
+  </si>
+  <si>
+    <t>AI Detect Jump</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that the opponent is an AI player </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> it is their turn </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> they should make jumps when available</t>
+    </r>
+  </si>
+  <si>
+    <t>Hint Detect Move</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that I don't know which move to make  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I click the hint button </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I expect to be told which moves are valid</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that is my turn </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I don't click the hint button  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I will not be told which moves are valid.</t>
+    </r>
+  </si>
+  <si>
+    <t>Highlight Hint</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>Given</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> that I need a hint </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>when</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> when I click the hint button </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+      </rPr>
+      <t>then</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> I except the board to highlight all valid moves</t>
+    </r>
+  </si>
+  <si>
+    <t>SQ 11/24</t>
+  </si>
+  <si>
+    <t>SQ 11/23</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -309,6 +955,16 @@
       <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -380,7 +1036,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -412,9 +1068,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -461,99 +1114,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="38">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="40">
     <dxf>
       <fill>
         <patternFill>
@@ -691,6 +1263,20 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color rgb="FF9C0006"/>
       </font>
@@ -707,6 +1293,54 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -775,6 +1409,34 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1175,9 +1837,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V592"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1238,7 +1900,12 @@
       <c r="F2" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G2" s="8"/>
+      <c r="G2" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="3" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="7"/>
@@ -1257,7 +1924,12 @@
       <c r="F3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G3" s="8"/>
+      <c r="G3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="4" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="7"/>
@@ -1276,7 +1948,12 @@
       <c r="F4" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="8"/>
+      <c r="G4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="64" x14ac:dyDescent="0.2">
       <c r="A5" s="7"/>
@@ -1295,7 +1972,12 @@
       <c r="F5" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G5" s="8"/>
+      <c r="G5" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
@@ -1314,7 +1996,12 @@
       <c r="F6" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G6" s="8"/>
+      <c r="G6" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="7" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
@@ -1333,7 +2020,12 @@
       <c r="F7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G7" s="8"/>
+      <c r="G7" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="8" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A8" s="7"/>
@@ -1352,7 +2044,12 @@
       <c r="F8" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G8" s="8"/>
+      <c r="G8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A9" s="7"/>
@@ -1371,7 +2068,12 @@
       <c r="F9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G9" s="8"/>
+      <c r="G9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="10" spans="1:8" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="7"/>
@@ -1390,7 +2092,12 @@
       <c r="F10" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G10" s="8"/>
+      <c r="G10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="11" spans="1:8" ht="42" x14ac:dyDescent="0.15">
       <c r="A11" s="10" t="s">
@@ -1402,17 +2109,21 @@
       <c r="C11" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="15" t="s">
         <v>31</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G11" s="12"/>
-      <c r="H11" s="11"/>
+      <c r="G11" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
@@ -1422,16 +2133,21 @@
       <c r="C12" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="18" t="s">
+      <c r="D12" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E12" s="20" t="s">
+      <c r="E12" s="19" t="s">
         <v>31</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G12" s="8"/>
+      <c r="G12" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="13" spans="1:8" ht="48" x14ac:dyDescent="0.2">
       <c r="A13" s="7"/>
@@ -1441,16 +2157,21 @@
       <c r="C13" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="19" t="s">
+      <c r="D13" s="18" t="s">
         <v>51</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="20" t="s">
         <v>31</v>
       </c>
       <c r="F13" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G13" s="8"/>
+      <c r="G13" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="14" spans="1:8" ht="96" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
@@ -1460,16 +2181,21 @@
       <c r="C14" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D14" s="18" t="s">
+      <c r="D14" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="20" t="s">
         <v>31</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G14" s="8"/>
+      <c r="G14" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="7"/>
@@ -1479,16 +2205,21 @@
       <c r="C15" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="18" t="s">
+      <c r="D15" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E15" s="20" t="s">
+      <c r="E15" s="19" t="s">
         <v>31</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G15" s="8"/>
+      <c r="G15" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="16" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="7"/>
@@ -1498,16 +2229,21 @@
       <c r="C16" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="19" t="s">
         <v>31</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="8"/>
+      <c r="G16" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="17" spans="1:22" ht="64" x14ac:dyDescent="0.2">
       <c r="A17" s="7"/>
@@ -1517,16 +2253,21 @@
       <c r="C17" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="E17" s="20" t="s">
+      <c r="E17" s="19" t="s">
         <v>31</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G17" s="8"/>
+      <c r="G17" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="18" spans="1:22" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="7"/>
@@ -1536,16 +2277,21 @@
       <c r="C18" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="12" t="s">
         <v>51</v>
       </c>
-      <c r="E18" s="14" t="s">
+      <c r="E18" s="13" t="s">
         <v>31</v>
       </c>
       <c r="F18" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="8"/>
+      <c r="G18" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="19" spans="1:22" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
@@ -1558,13 +2304,18 @@
       <c r="D19" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E19" s="14" t="s">
+      <c r="E19" s="13" t="s">
         <v>31</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G19" s="8"/>
+      <c r="G19" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="20" spans="1:22" ht="32" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
@@ -1574,13 +2325,18 @@
       <c r="D20" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E20" s="14" t="s">
+      <c r="E20" s="13" t="s">
         <v>31</v>
       </c>
       <c r="F20" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G20" s="8"/>
+      <c r="G20" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="21" spans="1:22" ht="32" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
@@ -1590,13 +2346,18 @@
       <c r="D21" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E21" s="14" t="s">
+      <c r="E21" s="13" t="s">
         <v>31</v>
       </c>
       <c r="F21" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G21" s="8"/>
+      <c r="G21" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="22" spans="1:22" ht="32" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
@@ -1606,127 +2367,156 @@
       <c r="D22" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E22" s="14" t="s">
+      <c r="E22" s="13" t="s">
         <v>31</v>
       </c>
       <c r="F22" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G22" s="8"/>
+      <c r="G22" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="23" spans="1:22" ht="32" x14ac:dyDescent="0.2">
-      <c r="A23" s="17"/>
-      <c r="B23" s="17" t="s">
+      <c r="A23" s="16"/>
+      <c r="B23" s="16" t="s">
         <v>37</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E23" s="14" t="s">
+      <c r="E23" s="13" t="s">
         <v>31</v>
       </c>
       <c r="F23" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G23" s="8"/>
+      <c r="G23" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="24" spans="1:22" ht="48" x14ac:dyDescent="0.2">
-      <c r="A24" s="24" t="s">
+      <c r="A24" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B24" s="24" t="s">
+      <c r="B24" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C24" s="25"/>
-      <c r="D24" s="22" t="s">
+      <c r="C24" s="24"/>
+      <c r="D24" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="E24" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F24" s="22" t="s">
+      <c r="E24" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F24" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="G24" s="25"/>
-      <c r="H24" s="22"/>
-      <c r="I24" s="26"/>
-      <c r="J24" s="26"/>
-      <c r="K24" s="26"/>
-      <c r="L24" s="26"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="26"/>
-      <c r="O24" s="26"/>
-      <c r="P24" s="26"/>
-      <c r="Q24" s="26"/>
-      <c r="R24" s="26"/>
-      <c r="S24" s="26"/>
-      <c r="T24" s="26"/>
-      <c r="U24" s="26"/>
-      <c r="V24" s="26"/>
+      <c r="G24" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I24" s="25"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="25"/>
+      <c r="N24" s="25"/>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="25"/>
+      <c r="S24" s="25"/>
+      <c r="T24" s="25"/>
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
     </row>
     <row r="25" spans="1:22" ht="48" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="17" t="s">
         <v>41</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E25" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F25" s="22" t="s">
+      <c r="E25" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F25" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="G25" s="8"/>
+      <c r="G25" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="26" spans="1:22" ht="80" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="17" t="s">
         <v>43</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E26" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F26" s="22" t="s">
+      <c r="E26" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="G26" s="8"/>
+      <c r="G26" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="27" spans="1:22" ht="48" x14ac:dyDescent="0.2">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="17" t="s">
         <v>44</v>
       </c>
-      <c r="B27" s="18" t="s">
+      <c r="B27" s="17" t="s">
         <v>45</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="14" t="s">
-        <v>31</v>
-      </c>
-      <c r="F27" s="22" t="s">
+      <c r="E27" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="F27" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="G27" s="8"/>
+      <c r="G27" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="28" spans="1:22" ht="64" x14ac:dyDescent="0.2">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="B28" s="13" t="s">
+      <c r="B28" s="12" t="s">
         <v>48</v>
       </c>
       <c r="C28" s="8"/>
@@ -1739,11 +2529,16 @@
       <c r="F28" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G28" s="8"/>
+      <c r="G28" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="29" spans="1:22" ht="32" x14ac:dyDescent="0.2">
-      <c r="A29" s="18"/>
-      <c r="B29" s="18" t="s">
+      <c r="A29" s="17"/>
+      <c r="B29" s="17" t="s">
         <v>49</v>
       </c>
       <c r="C29" s="8"/>
@@ -1756,13 +2551,18 @@
       <c r="F29" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="G29" s="8"/>
+      <c r="G29" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="30" spans="1:22" ht="96" x14ac:dyDescent="0.2">
-      <c r="A30" s="23" t="s">
+      <c r="A30" s="22" t="s">
         <v>55</v>
       </c>
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="22" t="s">
         <v>56</v>
       </c>
       <c r="C30" s="8"/>
@@ -1775,11 +2575,16 @@
       <c r="F30" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G30" s="8"/>
+      <c r="G30" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="31" spans="1:22" ht="32" x14ac:dyDescent="0.2">
-      <c r="A31" s="24"/>
-      <c r="B31" s="24" t="s">
+      <c r="A31" s="23"/>
+      <c r="B31" s="23" t="s">
         <v>57</v>
       </c>
       <c r="C31" s="8"/>
@@ -1792,13 +2597,18 @@
       <c r="F31" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="G31" s="8"/>
+      <c r="G31" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="32" spans="1:22" ht="64" x14ac:dyDescent="0.2">
-      <c r="A32" s="27" t="s">
+      <c r="A32" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="B32" s="27" t="s">
+      <c r="B32" s="26" t="s">
         <v>59</v>
       </c>
       <c r="C32" s="8"/>
@@ -1811,11 +2621,16 @@
       <c r="F32" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G32" s="8"/>
-    </row>
-    <row r="33" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13" t="s">
+      <c r="G32" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12" t="s">
         <v>60</v>
       </c>
       <c r="C33" s="8"/>
@@ -1828,11 +2643,16 @@
       <c r="F33" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G33" s="8"/>
-    </row>
-    <row r="34" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A34" s="18"/>
-      <c r="B34" s="18" t="s">
+      <c r="G33" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A34" s="17"/>
+      <c r="B34" s="17" t="s">
         <v>61</v>
       </c>
       <c r="C34" s="8"/>
@@ -1845,13 +2665,18 @@
       <c r="F34" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G34" s="8"/>
-    </row>
-    <row r="35" spans="1:7" ht="80" x14ac:dyDescent="0.2">
-      <c r="A35" s="27" t="s">
+      <c r="G34" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="80" x14ac:dyDescent="0.2">
+      <c r="A35" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B35" s="27" t="s">
+      <c r="B35" s="26" t="s">
         <v>63</v>
       </c>
       <c r="C35" s="8"/>
@@ -1864,11 +2689,16 @@
       <c r="F35" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G35" s="8"/>
-    </row>
-    <row r="36" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A36" s="18"/>
-      <c r="B36" s="18" t="s">
+      <c r="G35" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A36" s="17"/>
+      <c r="B36" s="17" t="s">
         <v>64</v>
       </c>
       <c r="C36" s="8"/>
@@ -1881,13 +2711,18 @@
       <c r="F36" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="G36" s="8"/>
-    </row>
-    <row r="37" spans="1:7" ht="64" x14ac:dyDescent="0.2">
-      <c r="A37" s="13" t="s">
+      <c r="G36" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="64" x14ac:dyDescent="0.2">
+      <c r="A37" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="B37" s="13" t="s">
+      <c r="B37" s="12" t="s">
         <v>66</v>
       </c>
       <c r="C37" s="8"/>
@@ -1900,11 +2735,16 @@
       <c r="F37" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G37" s="8"/>
-    </row>
-    <row r="38" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13" t="s">
+      <c r="G37" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12" t="s">
         <v>67</v>
       </c>
       <c r="C38" s="8"/>
@@ -1917,11 +2757,16 @@
       <c r="F38" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G38" s="8"/>
-    </row>
-    <row r="39" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A39" s="13"/>
-      <c r="B39" s="13" t="s">
+      <c r="G38" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A39" s="12"/>
+      <c r="B39" s="12" t="s">
         <v>68</v>
       </c>
       <c r="C39" s="8"/>
@@ -1934,11 +2779,16 @@
       <c r="F39" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G39" s="8"/>
-    </row>
-    <row r="40" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13" t="s">
+      <c r="G39" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12" t="s">
         <v>69</v>
       </c>
       <c r="C40" s="8"/>
@@ -1951,11 +2801,16 @@
       <c r="F40" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G40" s="8"/>
-    </row>
-    <row r="41" spans="1:7" ht="32" x14ac:dyDescent="0.2">
-      <c r="A41" s="18"/>
-      <c r="B41" s="18" t="s">
+      <c r="G40" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A41" s="17"/>
+      <c r="B41" s="17" t="s">
         <v>70</v>
       </c>
       <c r="C41" s="8"/>
@@ -1968,13 +2823,18 @@
       <c r="F41" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="G41" s="8"/>
-    </row>
-    <row r="42" spans="1:7" ht="48" x14ac:dyDescent="0.2">
-      <c r="A42" s="19" t="s">
+      <c r="G41" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H41" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="48" x14ac:dyDescent="0.2">
+      <c r="A42" s="18" t="s">
         <v>71</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="18" t="s">
         <v>72</v>
       </c>
       <c r="C42" s="8"/>
@@ -1987,114 +2847,222 @@
       <c r="F42" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="G42" s="8"/>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G42" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H42" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A43" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" s="27" t="s">
+        <v>82</v>
+      </c>
       <c r="C43" s="8"/>
       <c r="E43" s="8"/>
-      <c r="G43" s="8"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G43" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H43" s="29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A44" s="21"/>
+      <c r="B44" s="27" t="s">
+        <v>83</v>
+      </c>
       <c r="C44" s="8"/>
       <c r="E44" s="8"/>
-      <c r="G44" s="8"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G44" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H44" s="29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A45" s="21"/>
+      <c r="B45" s="27" t="s">
+        <v>84</v>
+      </c>
       <c r="C45" s="8"/>
       <c r="E45" s="8"/>
-      <c r="G45" s="8"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G45" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H45" s="29" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="21"/>
+      <c r="B46" s="27"/>
       <c r="C46" s="8"/>
       <c r="E46" s="8"/>
       <c r="G46" s="8"/>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A47" s="21" t="s">
+        <v>85</v>
+      </c>
+      <c r="B47" s="27" t="s">
+        <v>86</v>
+      </c>
       <c r="C47" s="8"/>
       <c r="E47" s="8"/>
-      <c r="G47" s="8"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="G47" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="21"/>
+      <c r="B48" s="27"/>
       <c r="C48" s="8"/>
       <c r="E48" s="8"/>
       <c r="G48" s="8"/>
     </row>
-    <row r="49" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A49" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B49" s="27" t="s">
+        <v>86</v>
+      </c>
       <c r="C49" s="8"/>
       <c r="E49" s="8"/>
-      <c r="G49" s="8"/>
-    </row>
-    <row r="50" spans="3:7" x14ac:dyDescent="0.2">
+      <c r="G49" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" s="28"/>
+      <c r="B50" s="27"/>
       <c r="C50" s="8"/>
       <c r="E50" s="8"/>
       <c r="G50" s="8"/>
     </row>
-    <row r="51" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A51" s="21" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="27" t="s">
+        <v>89</v>
+      </c>
       <c r="C51" s="8"/>
       <c r="E51" s="8"/>
       <c r="G51" s="8"/>
     </row>
-    <row r="52" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A52" s="21"/>
+      <c r="B52" s="27" t="s">
+        <v>90</v>
+      </c>
       <c r="C52" s="8"/>
       <c r="E52" s="8"/>
       <c r="G52" s="8"/>
     </row>
-    <row r="53" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="21"/>
+      <c r="B53" s="27"/>
       <c r="C53" s="8"/>
       <c r="E53" s="8"/>
       <c r="G53" s="8"/>
     </row>
-    <row r="54" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A54" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B54" s="27" t="s">
+        <v>92</v>
+      </c>
       <c r="C54" s="8"/>
       <c r="E54" s="8"/>
       <c r="G54" s="8"/>
     </row>
-    <row r="55" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="21"/>
+      <c r="B55" s="27"/>
       <c r="C55" s="8"/>
       <c r="E55" s="8"/>
       <c r="G55" s="8"/>
     </row>
-    <row r="56" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A56" s="21" t="s">
+        <v>93</v>
+      </c>
+      <c r="B56" s="27" t="s">
+        <v>94</v>
+      </c>
       <c r="C56" s="8"/>
       <c r="E56" s="8"/>
       <c r="G56" s="8"/>
     </row>
-    <row r="57" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="21"/>
+      <c r="B57" s="27"/>
       <c r="C57" s="8"/>
       <c r="E57" s="8"/>
       <c r="G57" s="8"/>
     </row>
-    <row r="58" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A58" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" s="27" t="s">
+        <v>96</v>
+      </c>
       <c r="C58" s="8"/>
       <c r="E58" s="8"/>
       <c r="G58" s="8"/>
     </row>
-    <row r="59" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A59" s="21"/>
+      <c r="B59" s="27" t="s">
+        <v>97</v>
+      </c>
       <c r="C59" s="8"/>
       <c r="E59" s="8"/>
       <c r="G59" s="8"/>
     </row>
-    <row r="60" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="21"/>
+      <c r="B60" s="27"/>
       <c r="C60" s="8"/>
       <c r="E60" s="8"/>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:8" ht="32" x14ac:dyDescent="0.2">
+      <c r="A61" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="B61" s="27" t="s">
+        <v>99</v>
+      </c>
       <c r="C61" s="8"/>
       <c r="E61" s="8"/>
       <c r="G61" s="8"/>
     </row>
-    <row r="62" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C62" s="8"/>
       <c r="E62" s="8"/>
       <c r="G62" s="8"/>
     </row>
-    <row r="63" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C63" s="8"/>
       <c r="E63" s="8"/>
       <c r="G63" s="8"/>
     </row>
-    <row r="64" spans="3:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C64" s="8"/>
       <c r="E64" s="8"/>
       <c r="G64" s="8"/>
@@ -4740,24 +5708,24 @@
       <c r="G592" s="8"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="G2:G592 C2:C592 E2:E592">
-    <cfRule type="cellIs" dxfId="35" priority="11" operator="equal">
+  <conditionalFormatting sqref="C2:C592 E2:E592 G2:G592">
+    <cfRule type="cellIs" dxfId="27" priority="11" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H592 D2:D592 F2:F18 F24:F592">
-    <cfRule type="expression" dxfId="33" priority="5" stopIfTrue="1">
+  <conditionalFormatting sqref="D2:D592 F2:F18 F24:F592 H2:H592">
+    <cfRule type="expression" dxfId="25" priority="5" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="6" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C592 G2:G592 E2:E592">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C592 E2:E592 G2:G592">
       <formula1>"Pass,Fail"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
updated accpetance test plan
</commit_message>
<xml_diff>
--- a/etc/term-2181-swen-261-11-d.xlsx
+++ b/etc/term-2181-swen-261-11-d.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2440" yWindow="460" windowWidth="26300" windowHeight="16660" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="880" yWindow="460" windowWidth="26300" windowHeight="15580" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="106">
   <si>
     <t>Instructions</t>
   </si>
@@ -858,69 +858,28 @@
     </r>
   </si>
   <si>
-    <t>Highlight Hint</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>Given</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> that I need a hint </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>when</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> when I click the hint button </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-      </rPr>
-      <t>then</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> I except the board to highlight all valid moves</t>
-    </r>
-  </si>
-  <si>
     <t>SQ 11/24</t>
   </si>
   <si>
     <t>SQ 11/23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ZM 11/23</t>
+  </si>
+  <si>
+    <t>SF 11/23</t>
+  </si>
+  <si>
+    <t>JK 11/23</t>
+  </si>
+  <si>
+    <t>NS 11/23</t>
+  </si>
+  <si>
+    <t>ZM 11/23</t>
+  </si>
+  <si>
+    <t>ZM 11/26</t>
   </si>
 </sst>
 </file>
@@ -1125,7 +1084,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="40">
+  <dxfs count="26">
     <dxf>
       <fill>
         <patternFill>
@@ -1137,114 +1096,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1277,26 +1128,6 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
@@ -1307,60 +1138,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1393,22 +1170,58 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1837,9 +1650,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V592"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A48" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="H45" sqref="H45"/>
+    <sheetView tabSelected="1" topLeftCell="A30" zoomScale="125" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="H60" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1904,7 +1717,7 @@
         <v>31</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -1928,7 +1741,7 @@
         <v>31</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -1952,7 +1765,7 @@
         <v>31</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="64" x14ac:dyDescent="0.2">
@@ -1976,7 +1789,7 @@
         <v>31</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -2122,7 +1935,7 @@
         <v>31</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -2146,7 +1959,7 @@
         <v>31</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -2170,7 +1983,7 @@
         <v>31</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="96" x14ac:dyDescent="0.2">
@@ -2194,7 +2007,7 @@
         <v>31</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2218,7 +2031,7 @@
         <v>31</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2242,7 +2055,7 @@
         <v>31</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="64" x14ac:dyDescent="0.2">
@@ -2266,7 +2079,7 @@
         <v>31</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="49" thickBot="1" x14ac:dyDescent="0.25">
@@ -2290,7 +2103,7 @@
         <v>31</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="48" x14ac:dyDescent="0.2">
@@ -2314,7 +2127,7 @@
         <v>31</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="32" x14ac:dyDescent="0.2">
@@ -2335,7 +2148,7 @@
         <v>31</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="32" x14ac:dyDescent="0.2">
@@ -2356,7 +2169,7 @@
         <v>31</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:22" ht="32" x14ac:dyDescent="0.2">
@@ -2377,7 +2190,7 @@
         <v>31</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="23" spans="1:22" ht="32" x14ac:dyDescent="0.2">
@@ -2399,7 +2212,7 @@
         <v>31</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="1:22" ht="48" x14ac:dyDescent="0.2">
@@ -2423,7 +2236,7 @@
         <v>31</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="I24" s="25"/>
       <c r="J24" s="25"/>
@@ -2461,7 +2274,7 @@
         <v>31</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:22" ht="80" x14ac:dyDescent="0.2">
@@ -2485,7 +2298,7 @@
         <v>31</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:22" ht="48" x14ac:dyDescent="0.2">
@@ -2509,7 +2322,7 @@
         <v>31</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:22" ht="64" x14ac:dyDescent="0.2">
@@ -2533,7 +2346,7 @@
         <v>31</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:22" ht="32" x14ac:dyDescent="0.2">
@@ -2555,7 +2368,7 @@
         <v>31</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="30" spans="1:22" ht="96" x14ac:dyDescent="0.2">
@@ -2579,7 +2392,7 @@
         <v>31</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="31" spans="1:22" ht="32" x14ac:dyDescent="0.2">
@@ -2601,7 +2414,7 @@
         <v>31</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="32" spans="1:22" ht="64" x14ac:dyDescent="0.2">
@@ -2625,7 +2438,7 @@
         <v>31</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2647,7 +2460,7 @@
         <v>31</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2669,7 +2482,7 @@
         <v>31</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="80" x14ac:dyDescent="0.2">
@@ -2693,7 +2506,7 @@
         <v>31</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2715,7 +2528,7 @@
         <v>31</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="64" x14ac:dyDescent="0.2">
@@ -2739,7 +2552,7 @@
         <v>31</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2761,7 +2574,7 @@
         <v>31</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2783,7 +2596,7 @@
         <v>31</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2805,7 +2618,7 @@
         <v>31</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2827,7 +2640,7 @@
         <v>31</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="48" x14ac:dyDescent="0.2">
@@ -2851,7 +2664,7 @@
         <v>31</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2867,7 +2680,7 @@
         <v>31</v>
       </c>
       <c r="H43" s="29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2881,7 +2694,7 @@
         <v>31</v>
       </c>
       <c r="H44" s="29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="32" x14ac:dyDescent="0.2">
@@ -2895,7 +2708,7 @@
         <v>31</v>
       </c>
       <c r="H45" s="29" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.2">
@@ -2918,7 +2731,7 @@
         <v>31</v>
       </c>
       <c r="H47" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.2">
@@ -2941,7 +2754,7 @@
         <v>31</v>
       </c>
       <c r="H49" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.2">
@@ -2960,7 +2773,12 @@
       </c>
       <c r="C51" s="8"/>
       <c r="E51" s="8"/>
-      <c r="G51" s="8"/>
+      <c r="G51" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H51" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="52" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="21"/>
@@ -2969,7 +2787,12 @@
       </c>
       <c r="C52" s="8"/>
       <c r="E52" s="8"/>
-      <c r="G52" s="8"/>
+      <c r="G52" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H52" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="21"/>
@@ -2987,7 +2810,12 @@
       </c>
       <c r="C54" s="8"/>
       <c r="E54" s="8"/>
-      <c r="G54" s="8"/>
+      <c r="G54" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A55" s="21"/>
@@ -3005,7 +2833,12 @@
       </c>
       <c r="C56" s="8"/>
       <c r="E56" s="8"/>
-      <c r="G56" s="8"/>
+      <c r="G56" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H56" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A57" s="21"/>
@@ -3023,7 +2856,12 @@
       </c>
       <c r="C58" s="8"/>
       <c r="E58" s="8"/>
-      <c r="G58" s="8"/>
+      <c r="G58" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H58" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="59" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="21"/>
@@ -3032,7 +2870,12 @@
       </c>
       <c r="C59" s="8"/>
       <c r="E59" s="8"/>
-      <c r="G59" s="8"/>
+      <c r="G59" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A60" s="21"/>
@@ -3041,13 +2884,9 @@
       <c r="E60" s="8"/>
       <c r="G60" s="8"/>
     </row>
-    <row r="61" spans="1:8" ht="32" x14ac:dyDescent="0.2">
-      <c r="A61" s="21" t="s">
-        <v>98</v>
-      </c>
-      <c r="B61" s="27" t="s">
-        <v>99</v>
-      </c>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="21"/>
+      <c r="B61" s="27"/>
       <c r="C61" s="8"/>
       <c r="E61" s="8"/>
       <c r="G61" s="8"/>
@@ -5709,18 +5548,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C592 E2:E592 G2:G592">
-    <cfRule type="cellIs" dxfId="27" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="11" operator="equal">
       <formula>"Pass"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="12" operator="equal">
       <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D592 F2:F18 F24:F592 H2:H592">
-    <cfRule type="expression" dxfId="25" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="5" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Pass")</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="6" stopIfTrue="1">
       <formula>AND(ISBLANK(D2),C2="Fail")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>